<commit_message>
alpha version of pz
</commit_message>
<xml_diff>
--- a/excel/matr.xlsx
+++ b/excel/matr.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="97">
   <si>
     <t>{1}</t>
   </si>
@@ -198,36 +198,12 @@
     <t>sigma1^4</t>
   </si>
   <si>
-    <t>x12</t>
-  </si>
-  <si>
-    <t>x13</t>
-  </si>
-  <si>
-    <t>x14</t>
-  </si>
-  <si>
-    <t>x15</t>
-  </si>
-  <si>
-    <t>x16</t>
-  </si>
-  <si>
-    <t>x17</t>
-  </si>
-  <si>
-    <t>x18</t>
-  </si>
-  <si>
     <t>sigma5</t>
   </si>
   <si>
     <t>sigma4*sigma1</t>
   </si>
   <si>
-    <t>sigma3*sigma3</t>
-  </si>
-  <si>
     <t>sigma3*(sigma1^2)</t>
   </si>
   <si>
@@ -244,6 +220,96 @@
   </si>
   <si>
     <t>"</t>
+  </si>
+  <si>
+    <t>eq1:=1*x1+0*x2+0*x3+0=sigma1:</t>
+  </si>
+  <si>
+    <t>eq2:=0*x1+1*x2+1*x3+0=sigma2:</t>
+  </si>
+  <si>
+    <t>eq3:=0*x1+3*x2+2*x3+10=(sigma1)^2:</t>
+  </si>
+  <si>
+    <t>eq1:=1*x1+0*x2+0*x3+0*x4+0*x5+0*x6+0=sigma1:</t>
+  </si>
+  <si>
+    <t>eq2:=0*x1+1*x2+1*x3+0*x4+0*x5+0*x6+0=sigma2:</t>
+  </si>
+  <si>
+    <t>eq3:=0*x1+3*x2+2*x3+0*x4+0*x5+0*x6+21=sigma1^2:</t>
+  </si>
+  <si>
+    <t>eq4:=0*x1+0*x2+0*x3+1*x4+1*x5+1*x6+0=sigma3:</t>
+  </si>
+  <si>
+    <t>eq5:=20*x1+0*x2+0*x3+6*x4+4*x5+3*x6+0=sigma2*sigma1:</t>
+  </si>
+  <si>
+    <t>eq6:=71*x1+0*x2+0*x3+16*x4+9*x5+6*x6+0=sigma1^3:</t>
+  </si>
+  <si>
+    <t>eq11:=0*x1+783*x2+544*x3+0*x4+0*x5+0*x6+125*x7+64*x8+54*x9+36*x10+24*x11+4320=sigma1^4:</t>
+  </si>
+  <si>
+    <t>x_1</t>
+  </si>
+  <si>
+    <t>x_2</t>
+  </si>
+  <si>
+    <t>x_3</t>
+  </si>
+  <si>
+    <t>x_4</t>
+  </si>
+  <si>
+    <t>x_5</t>
+  </si>
+  <si>
+    <t>x_6</t>
+  </si>
+  <si>
+    <t>x_7</t>
+  </si>
+  <si>
+    <t>x_8</t>
+  </si>
+  <si>
+    <t>x_9</t>
+  </si>
+  <si>
+    <t>x_10</t>
+  </si>
+  <si>
+    <t>x_11</t>
+  </si>
+  <si>
+    <t>x_12</t>
+  </si>
+  <si>
+    <t>x_13</t>
+  </si>
+  <si>
+    <t>x_14</t>
+  </si>
+  <si>
+    <t>x_15</t>
+  </si>
+  <si>
+    <t>x_16</t>
+  </si>
+  <si>
+    <t>x_17</t>
+  </si>
+  <si>
+    <t>x_18</t>
+  </si>
+  <si>
+    <t>sigma3*sigma2</t>
+  </si>
+  <si>
+    <t>eq18:=60121*x_1+0*x_2+0*x_3+11168*x_4+6681*x_5+4500*x_6+0*x_7+0*x_8+0*x_9+0*x_10+0*x_11+1296*x_12+625*x_13+480*x_14+320*x_15+270*x_16+180*x_17+120*x_18+0=(sigma1^5):</t>
   </si>
 </sst>
 </file>
@@ -581,7 +647,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -614,10 +680,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Лист2"/>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -712,7 +778,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -736,7 +802,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C7">
         <f>MDETERM(E3:G5)</f>
@@ -753,6 +819,21 @@
       <c r="G7" t="str">
         <f t="shared" si="1"/>
         <v>x3:="(2,1)(4,3)":</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="I12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="I13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="I14" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -763,10 +844,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Лист3"/>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:J10"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -973,7 +1054,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -1042,7 +1123,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C10">
         <f>MDETERM(E3:J8)</f>
@@ -1071,6 +1152,36 @@
       <c r="J10" t="str">
         <f t="shared" si="1"/>
         <v>x6:="(2,1)(4,3)(6,5)":</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="L14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="L15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="L16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="12:12">
+      <c r="L17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="12:12">
+      <c r="L18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="12:12">
+      <c r="L19" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1081,10 +1192,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Лист4"/>
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1385,7 +1496,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -1739,7 +1850,7 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C15">
         <f>MDETERM(E3:O13)</f>
@@ -1788,6 +1899,11 @@
       <c r="O15" t="str">
         <f t="shared" si="1"/>
         <v>x11:="(2,1)(4,3)(6,5)(8,7)":</v>
+      </c>
+    </row>
+    <row r="17" spans="17:17">
+      <c r="Q17" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1799,10 +1915,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Лист5"/>
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3:X20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1829,58 +1945,58 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="E1" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="G1" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="I1" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="J1" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="K1" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="L1" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="M1" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="N1" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="O1" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="P1" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="Q1" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="R1" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="S1" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="T1" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="U1" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="V1" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1">
@@ -2011,7 +2127,7 @@
       </c>
       <c r="X3" t="str">
         <f>$B$1&amp;"eq"&amp;A3&amp;":="&amp;(E3&amp;"*"&amp;$E$1)&amp;"+"&amp;(F3&amp;"*"&amp;$F$1)&amp;"+"&amp;(G3&amp;"*"&amp;$G$1)&amp;"+"&amp;(H3&amp;"*"&amp;$H$1)&amp;"+"&amp;(I3&amp;"*"&amp;$I$1)&amp;"+"&amp;(J3&amp;"*"&amp;$J$1)&amp;"+"&amp;(K3&amp;"*"&amp;$K$1)&amp;"+"&amp;(L3&amp;"*"&amp;$L$1)&amp;"+"&amp;(M3&amp;"*"&amp;$M$1)&amp;"+"&amp;(N3&amp;"*"&amp;$N$1)&amp;"+"&amp;(O3&amp;"*"&amp;$O$1)&amp;"+"&amp;(P3&amp;"*"&amp;$P$1)&amp;"+"&amp;(Q3&amp;"*"&amp;$Q$1)&amp;"+"&amp;(R3&amp;"*"&amp;$R$1)&amp;"+"&amp;(S3&amp;"*"&amp;$S$1)&amp;"+"&amp;(T3&amp;"*"&amp;$T$1)&amp;"+"&amp;(U3&amp;"*"&amp;$U$1)&amp;"+"&amp;(V3&amp;"*"&amp;$V$1)&amp;"+"&amp;(D3)&amp;"="&amp;(B3)&amp;":"</f>
-        <v>eq1:=1*x1+0*x2+0*x3+0*x4+0*x5+0*x6+0*x7+0*x8+0*x9+0*x10+0*x11+0*x12+0*x13+0*x14+0*x15+0*x16+0*x17+0*x18+0=sigma1:</v>
+        <v>eq1:=1*x_1+0*x_2+0*x_3+0*x_4+0*x_5+0*x_6+0*x_7+0*x_8+0*x_9+0*x_10+0*x_11+0*x_12+0*x_13+0*x_14+0*x_15+0*x_16+0*x_17+0*x_18+0=sigma1:</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -2083,7 +2199,7 @@
       </c>
       <c r="X4" t="str">
         <f t="shared" ref="X4:X20" si="0">$B$1&amp;"eq"&amp;A4&amp;":="&amp;(E4&amp;"*"&amp;$E$1)&amp;"+"&amp;(F4&amp;"*"&amp;$F$1)&amp;"+"&amp;(G4&amp;"*"&amp;$G$1)&amp;"+"&amp;(H4&amp;"*"&amp;$H$1)&amp;"+"&amp;(I4&amp;"*"&amp;$I$1)&amp;"+"&amp;(J4&amp;"*"&amp;$J$1)&amp;"+"&amp;(K4&amp;"*"&amp;$K$1)&amp;"+"&amp;(L4&amp;"*"&amp;$L$1)&amp;"+"&amp;(M4&amp;"*"&amp;$M$1)&amp;"+"&amp;(N4&amp;"*"&amp;$N$1)&amp;"+"&amp;(O4&amp;"*"&amp;$O$1)&amp;"+"&amp;(P4&amp;"*"&amp;$P$1)&amp;"+"&amp;(Q4&amp;"*"&amp;$Q$1)&amp;"+"&amp;(R4&amp;"*"&amp;$R$1)&amp;"+"&amp;(S4&amp;"*"&amp;$S$1)&amp;"+"&amp;(T4&amp;"*"&amp;$T$1)&amp;"+"&amp;(U4&amp;"*"&amp;$U$1)&amp;"+"&amp;(V4&amp;"*"&amp;$V$1)&amp;"+"&amp;(D4)&amp;"="&amp;(B4)&amp;":"</f>
-        <v>eq2:=0*x1+1*x2+1*x3+0*x4+0*x5+0*x6+0*x7+0*x8+0*x9+0*x10+0*x11+0*x12+0*x13+0*x14+0*x15+0*x16+0*x17+0*x18+0=sigma2:</v>
+        <v>eq2:=0*x_1+1*x_2+1*x_3+0*x_4+0*x_5+0*x_6+0*x_7+0*x_8+0*x_9+0*x_10+0*x_11+0*x_12+0*x_13+0*x_14+0*x_15+0*x_16+0*x_17+0*x_18+0=sigma2:</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -2155,7 +2271,7 @@
       </c>
       <c r="X5" t="str">
         <f t="shared" si="0"/>
-        <v>eq3:=0*x1+3*x2+2*x3+0*x4+0*x5+0*x6+0*x7+0*x8+0*x9+0*x10+0*x11+0*x12+0*x13+0*x14+0*x15+0*x16+0*x17+0*x18+55=sigma1^2:</v>
+        <v>eq3:=0*x_1+3*x_2+2*x_3+0*x_4+0*x_5+0*x_6+0*x_7+0*x_8+0*x_9+0*x_10+0*x_11+0*x_12+0*x_13+0*x_14+0*x_15+0*x_16+0*x_17+0*x_18+55=sigma1^2:</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -2227,7 +2343,7 @@
       </c>
       <c r="X6" t="str">
         <f t="shared" si="0"/>
-        <v>eq4:=0*x1+0*x2+0*x3+1*x4+1*x5+1*x6+0*x7+0*x8+0*x9+0*x10+0*x11+0*x12+0*x13+0*x14+0*x15+0*x16+0*x17+0*x18+0=sigma3:</v>
+        <v>eq4:=0*x_1+0*x_2+0*x_3+1*x_4+1*x_5+1*x_6+0*x_7+0*x_8+0*x_9+0*x_10+0*x_11+0*x_12+0*x_13+0*x_14+0*x_15+0*x_16+0*x_17+0*x_18+0=sigma3:</v>
       </c>
     </row>
     <row r="7" spans="1:24">
@@ -2235,7 +2351,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -2299,7 +2415,7 @@
       </c>
       <c r="X7" t="str">
         <f t="shared" si="0"/>
-        <v>eq5:=54*x1+0*x2+0*x3+6*x4+4*x5+3*x6+0*x7+0*x8+0*x9+0*x10+0*x11+0*x12+0*x13+0*x14+0*x15+0*x16+0*x17+0*x18+0=sigma2*sigma1:</v>
+        <v>eq5:=54*x_1+0*x_2+0*x_3+6*x_4+4*x_5+3*x_6+0*x_7+0*x_8+0*x_9+0*x_10+0*x_11+0*x_12+0*x_13+0*x_14+0*x_15+0*x_16+0*x_17+0*x_18+0=sigma2*sigma1:</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -2371,7 +2487,7 @@
       </c>
       <c r="X8" t="str">
         <f t="shared" si="0"/>
-        <v>eq6:=181*x1+0*x2+0*x3+16*x4+9*x5+6*x6+0*x7+0*x8+0*x9+0*x10+0*x11+0*x12+0*x13+0*x14+0*x15+0*x16+0*x17+0*x18+0=sigma1^3:</v>
+        <v>eq6:=181*x_1+0*x_2+0*x_3+16*x_4+9*x_5+6*x_6+0*x_7+0*x_8+0*x_9+0*x_10+0*x_11+0*x_12+0*x_13+0*x_14+0*x_15+0*x_16+0*x_17+0*x_18+0=sigma1^3:</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -2443,7 +2559,7 @@
       </c>
       <c r="X9" t="str">
         <f t="shared" si="0"/>
-        <v>eq7:=0*x1+0*x2+0*x3+0*x4+0*x5+0*x6+1*x7+1*x8+1*x9+1*x10+1*x11+0*x12+0*x13+0*x14+0*x15+0*x16+0*x17+0*x18+0=sigma4:</v>
+        <v>eq7:=0*x_1+0*x_2+0*x_3+0*x_4+0*x_5+0*x_6+1*x_7+1*x_8+1*x_9+1*x_10+1*x_11+0*x_12+0*x_13+0*x_14+0*x_15+0*x_16+0*x_17+0*x_18+0=sigma4:</v>
       </c>
     </row>
     <row r="10" spans="1:24">
@@ -2515,7 +2631,7 @@
       </c>
       <c r="X10" t="str">
         <f t="shared" si="0"/>
-        <v>eq8:=0*x1+52*x2+53*x3+0*x4+0*x5+0*x6+10*x7+7*x8+6*x9+5*x10+4*x11+0*x12+0*x13+0*x14+0*x15+0*x16+0*x17+0*x18+0=sigma3*sigma1:</v>
+        <v>eq8:=0*x_1+52*x_2+53*x_3+0*x_4+0*x_5+0*x_6+10*x_7+7*x_8+6*x_9+5*x_10+4*x_11+0*x_12+0*x_13+0*x_14+0*x_15+0*x_16+0*x_17+0*x_18+0=sigma3*sigma1:</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -2587,7 +2703,7 @@
       </c>
       <c r="X11" t="str">
         <f t="shared" si="0"/>
-        <v>eq9:=0*x1+157*x2+108*x3+0*x4+0*x5+0*x6+20*x7+12*x8+11*x9+8*x10+6*x11+0*x12+0*x13+0*x14+0*x15+0*x16+0*x17+0*x18+1320=sigma2^2:</v>
+        <v>eq9:=0*x_1+157*x_2+108*x_3+0*x_4+0*x_5+0*x_6+20*x_7+12*x_8+11*x_9+8*x_10+6*x_11+0*x_12+0*x_13+0*x_14+0*x_15+0*x_16+0*x_17+0*x_18+1320=sigma2^2:</v>
       </c>
     </row>
     <row r="12" spans="1:24">
@@ -2659,7 +2775,7 @@
       </c>
       <c r="X12" t="str">
         <f t="shared" si="0"/>
-        <v>eq10:=0*x1+418*x2+307*x3+0*x4+0*x5+0*x6+50*x7+28*x8+24*x9+17*x10+12*x11+0*x12+0*x13+0*x14+0*x15+0*x16+0*x17+0*x18+2970=sigma2*(sigma1^2):</v>
+        <v>eq10:=0*x_1+418*x_2+307*x_3+0*x_4+0*x_5+0*x_6+50*x_7+28*x_8+24*x_9+17*x_10+12*x_11+0*x_12+0*x_13+0*x_14+0*x_15+0*x_16+0*x_17+0*x_18+2970=sigma2*(sigma1^2):</v>
       </c>
     </row>
     <row r="13" spans="1:24">
@@ -2731,7 +2847,7 @@
       </c>
       <c r="X13" t="str">
         <f t="shared" si="0"/>
-        <v>eq11:=0*x1+1179*x2+804*x3+0*x4+0*x5+0*x6+125*x7+64*x8+54*x9+36*x10+24*x11+0*x12+0*x13+0*x14+0*x15+0*x16+0*x17+0*x18+9955=sigma1^4:</v>
+        <v>eq11:=0*x_1+1179*x_2+804*x_3+0*x_4+0*x_5+0*x_6+125*x_7+64*x_8+54*x_9+36*x_10+24*x_11+0*x_12+0*x_13+0*x_14+0*x_15+0*x_16+0*x_17+0*x_18+9955=sigma1^4:</v>
       </c>
     </row>
     <row r="14" spans="1:24">
@@ -2739,7 +2855,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
         <v>23</v>
@@ -2803,7 +2919,7 @@
       </c>
       <c r="X14" t="str">
         <f t="shared" si="0"/>
-        <v>eq12:=0*x1+0*x2+0*x3+0*x4+0*x5+0*x6+0*x7+0*x8+0*x9+0*x10+0*x11+1*x12+1*x13+1*x14+1*x15+1*x16+1*x17+1*x18+0=sigma5:</v>
+        <v>eq12:=0*x_1+0*x_2+0*x_3+0*x_4+0*x_5+0*x_6+0*x_7+0*x_8+0*x_9+0*x_10+0*x_11+1*x_12+1*x_13+1*x_14+1*x_15+1*x_16+1*x_17+1*x_18+0=sigma5:</v>
       </c>
     </row>
     <row r="15" spans="1:24">
@@ -2811,7 +2927,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
@@ -2875,7 +2991,7 @@
       </c>
       <c r="X15" t="str">
         <f t="shared" si="0"/>
-        <v>eq13:=0*x1+0*x2+0*x3+49*x4+51*x5+0*x6+0*x7+0*x8+0*x9+52*x10+0*x11+15*x12+11*x13+9*x14+8*x15+7*x16+6*x17+5*x18+0=sigma4*sigma1:</v>
+        <v>eq13:=0*x_1+0*x_2+0*x_3+49*x_4+51*x_5+0*x_6+0*x_7+0*x_8+0*x_9+52*x_10+0*x_11+15*x_12+11*x_13+9*x_14+8*x_15+7*x_16+6*x_17+5*x_18+0=sigma4*sigma1:</v>
       </c>
     </row>
     <row r="16" spans="1:24">
@@ -2883,7 +2999,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
         <v>25</v>
@@ -2947,7 +3063,7 @@
       </c>
       <c r="X16" t="str">
         <f t="shared" si="0"/>
-        <v>eq14:=1266*x1+0*x2+0*x3+299*x4+211*x5+162*x6+0*x7+0*x8+0*x9+0*x10+0*x11+50*x12+30*x13+25*x14+19*x15+17*x16+13*x17+10*x18+0=sigma3*(sigma1^2):</v>
+        <v>eq14:=1266*x_1+0*x_2+0*x_3+299*x_4+211*x_5+162*x_6+0*x_7+0*x_8+0*x_9+0*x_10+0*x_11+50*x_12+30*x_13+25*x_14+19*x_15+17*x_16+13*x_17+10*x_18+0=sigma3*sigma2:</v>
       </c>
     </row>
     <row r="17" spans="1:24">
@@ -2955,7 +3071,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
@@ -3018,8 +3134,8 @@
         <v>20</v>
       </c>
       <c r="X17" t="str">
-        <f t="shared" si="0"/>
-        <v>eq15:=2844*x1+0*x2+0*x3+741*x4+544*x5+433*x6+0*x7+0*x8+0*x9+0*x10+0*x11+120*x12+70*x13+55*x14+42*x15+36*x16+27*x17+20*x18+0=sigma3*sigma3:</v>
+        <f>$B$1&amp;"eq"&amp;A17&amp;":="&amp;(E17&amp;"*"&amp;$E$1)&amp;"+"&amp;(F17&amp;"*"&amp;$F$1)&amp;"+"&amp;(G17&amp;"*"&amp;$G$1)&amp;"+"&amp;(H17&amp;"*"&amp;$H$1)&amp;"+"&amp;(I17&amp;"*"&amp;$I$1)&amp;"+"&amp;(J17&amp;"*"&amp;$J$1)&amp;"+"&amp;(K17&amp;"*"&amp;$K$1)&amp;"+"&amp;(L17&amp;"*"&amp;$L$1)&amp;"+"&amp;(M17&amp;"*"&amp;$M$1)&amp;"+"&amp;(N17&amp;"*"&amp;$N$1)&amp;"+"&amp;(O17&amp;"*"&amp;$O$1)&amp;"+"&amp;(P17&amp;"*"&amp;$P$1)&amp;"+"&amp;(Q17&amp;"*"&amp;$Q$1)&amp;"+"&amp;(R17&amp;"*"&amp;$R$1)&amp;"+"&amp;(S17&amp;"*"&amp;$S$1)&amp;"+"&amp;(T17&amp;"*"&amp;$T$1)&amp;"+"&amp;(U17&amp;"*"&amp;$U$1)&amp;"+"&amp;(V17&amp;"*"&amp;$V$1)&amp;"+"&amp;(D17)&amp;"="&amp;(B17)&amp;":"</f>
+        <v>eq15:=2844*x_1+0*x_2+0*x_3+741*x_4+544*x_5+433*x_6+0*x_7+0*x_8+0*x_9+0*x_10+0*x_11+120*x_12+70*x_13+55*x_14+42*x_15+36*x_16+27*x_17+20*x_18+0=sigma3*(sigma1^2):</v>
       </c>
     </row>
     <row r="18" spans="1:24">
@@ -3091,7 +3207,7 @@
       </c>
       <c r="X18" t="str">
         <f t="shared" si="0"/>
-        <v>eq16:=8034*x1+0*x2+0*x3+1656*x4+1069*x5+768*x6+0*x7+0*x8+0*x9+0*x10+0*x11+225*x12+120*x13+96*x14+68*x15+59*x16+42*x17+30*x18+0=(sigma2^2)*sigma1:</v>
+        <v>eq16:=8034*x_1+0*x_2+0*x_3+1656*x_4+1069*x_5+768*x_6+0*x_7+0*x_8+0*x_9+0*x_10+0*x_11+225*x_12+120*x_13+96*x_14+68*x_15+59*x_16+42*x_17+30*x_18+0=(sigma2^2)*sigma1:</v>
       </c>
     </row>
     <row r="19" spans="1:24">
@@ -3099,7 +3215,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
         <v>35</v>
@@ -3163,7 +3279,7 @@
       </c>
       <c r="X19" t="str">
         <f t="shared" si="0"/>
-        <v>eq17:=21546*x1+0*x2+0*x3+4274*x4+2686*x5+1887*x6+0*x7+0*x8+0*x9+0*x10+0*x11+540*x12+275*x13+214*x14+148*x15+126*x16+87*x17+60*x18+0=sigma2*(sigma1^3):</v>
+        <v>eq17:=21546*x_1+0*x_2+0*x_3+4274*x_4+2686*x_5+1887*x_6+0*x_7+0*x_8+0*x_9+0*x_10+0*x_11+540*x_12+275*x_13+214*x_14+148*x_15+126*x_16+87*x_17+60*x_18+0=sigma2*(sigma1^3):</v>
       </c>
     </row>
     <row r="20" spans="1:24">
@@ -3171,7 +3287,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
         <v>36</v>
@@ -3235,12 +3351,12 @@
       </c>
       <c r="X20" t="str">
         <f t="shared" si="0"/>
-        <v>eq18:=60121*x1+0*x2+0*x3+11168*x4+6681*x5+4500*x6+0*x7+0*x8+0*x9+0*x10+0*x11+1296*x12+625*x13+480*x14+320*x15+270*x16+180*x17+120*x18+0=(sigma1^5):</v>
+        <v>eq18:=60121*x_1+0*x_2+0*x_3+11168*x_4+6681*x_5+4500*x_6+0*x_7+0*x_8+0*x_9+0*x_10+0*x_11+1296*x_12+625*x_13+480*x_14+320*x_15+270*x_16+180*x_17+120*x_18+0=(sigma1^5):</v>
       </c>
     </row>
     <row r="22" spans="1:24">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C22">
         <f>MDETERM(E3:V20)</f>
@@ -3248,79 +3364,85 @@
       </c>
       <c r="E22" t="str">
         <f>(E1&amp;":="&amp;$A22&amp;""&amp;E2&amp;""&amp;$A22)&amp;":"</f>
-        <v>x1:="(2,1)":</v>
+        <v>x_1:="(2,1)":</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" ref="F22:V22" si="1">(F1&amp;":="&amp;$A22&amp;""&amp;F2&amp;""&amp;$A22)&amp;":"</f>
-        <v>x2:="(3,2,1)":</v>
+        <v>x_2:="(3,2,1)":</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
-        <v>x3:="(2,1)(4,3)":</v>
+        <v>x_3:="(2,1)(4,3)":</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="1"/>
-        <v>x4:="(4,3,2,1)":</v>
+        <v>x_4:="(4,3,2,1)":</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="1"/>
-        <v>x5:="(3,2,1)(5,4)":</v>
+        <v>x_5:="(3,2,1)(5,4)":</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="1"/>
-        <v>x6:="(2,1)(4,3)(6,5)":</v>
+        <v>x_6:="(2,1)(4,3)(6,5)":</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="1"/>
-        <v>x7:="(5,4,3,2,1)":</v>
+        <v>x_7:="(5,4,3,2,1)":</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="1"/>
-        <v>x8:="(4,3,2,1)(6,5)":</v>
+        <v>x_8:="(4,3,2,1)(6,5)":</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="1"/>
-        <v>x9:="(3,2,1)(6,5,4)":</v>
+        <v>x_9:="(3,2,1)(6,5,4)":</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" si="1"/>
-        <v>x10:="(3,2,1)(5,4)(7,6)":</v>
+        <v>x_10:="(3,2,1)(5,4)(7,6)":</v>
       </c>
       <c r="O22" t="str">
         <f t="shared" si="1"/>
-        <v>x11:="(2,1)(4,3)(6,5)(8,7)":</v>
+        <v>x_11:="(2,1)(4,3)(6,5)(8,7)":</v>
       </c>
       <c r="P22" t="str">
         <f t="shared" si="1"/>
-        <v>x12:="(6,5,4,3,2,1)":</v>
+        <v>x_12:="(6,5,4,3,2,1)":</v>
       </c>
       <c r="Q22" t="str">
         <f t="shared" si="1"/>
-        <v>x13:="(5,4,3,2,1)(7,6)":</v>
+        <v>x_13:="(5,4,3,2,1)(7,6)":</v>
       </c>
       <c r="R22" t="str">
         <f t="shared" si="1"/>
-        <v>x14:="(4,3,2,1)(7,6,5)":</v>
+        <v>x_14:="(4,3,2,1)(7,6,5)":</v>
       </c>
       <c r="S22" t="str">
         <f t="shared" si="1"/>
-        <v>x15:="(4,3,2,1)(6,5)(8,7)":</v>
+        <v>x_15:="(4,3,2,1)(6,5)(8,7)":</v>
       </c>
       <c r="T22" t="str">
         <f t="shared" si="1"/>
-        <v>x16:="(3,2,1)(6,5,4)(8,7)":</v>
+        <v>x_16:="(3,2,1)(6,5,4)(8,7)":</v>
       </c>
       <c r="U22" t="str">
         <f t="shared" si="1"/>
-        <v>x17:="(3,2,1)(5,4)(7,6)(9,8)":</v>
+        <v>x_17:="(3,2,1)(5,4)(7,6)(9,8)":</v>
       </c>
       <c r="V22" t="str">
         <f t="shared" si="1"/>
-        <v>x18:="(2,1)(4,3)(6,5)(8,7)(10,9)":</v>
+        <v>x_18:="(2,1)(4,3)(6,5)(8,7)(10,9)":</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24">
+      <c r="X23" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
PZ again + scilab fail
</commit_message>
<xml_diff>
--- a/excel/matr.xlsx
+++ b/excel/matr.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="106">
   <si>
     <t>{1}</t>
   </si>
@@ -310,6 +310,33 @@
   </si>
   <si>
     <t>eq18:=60121*x_1+0*x_2+0*x_3+11168*x_4+6681*x_5+4500*x_6+0*x_7+0*x_8+0*x_9+0*x_10+0*x_11+1296*x_12+625*x_13+480*x_14+320*x_15+270*x_16+180*x_17+120*x_18+0=(sigma1^5):</t>
+  </si>
+  <si>
+    <t>1*x1+0*x2+0*x3+0*x4+0*x5+0*x6+0=sigma1:</t>
+  </si>
+  <si>
+    <t>0*x1+1*x2+1*x3+0*x4+0*x5+0*x6+0=sigma2:</t>
+  </si>
+  <si>
+    <t>0*x1+3*x2+2*x3+0*x4+0*x5+0*x6+21=sigma1^2:</t>
+  </si>
+  <si>
+    <t>0*x1+0*x2+0*x3+1*x4+1*x5+1*x6+0=sigma3:</t>
+  </si>
+  <si>
+    <t>20*x1+0*x2+0*x3+6*x4+4*x5+3*x6+0=sigma2*sigma1:</t>
+  </si>
+  <si>
+    <t>71*x1+0*x2+0*x3+16*x4+9*x5+6*x6+0=sigma1^3:</t>
+  </si>
+  <si>
+    <t>1*x(1)+0*x(2)+0*x(3)+0=sigma1:</t>
+  </si>
+  <si>
+    <t>0*x(1)+1*x(2)+1*x(3)+0=sigma2:</t>
+  </si>
+  <si>
+    <t>0*x(1)+3*x(2)+2*x(3)+10=(sigma1)^2:</t>
   </si>
 </sst>
 </file>
@@ -682,8 +709,8 @@
   <sheetPr codeName="Лист2"/>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -822,22 +849,32 @@
       </c>
     </row>
     <row r="12" spans="1:9">
+      <c r="E12" t="s">
+        <v>103</v>
+      </c>
       <c r="I12" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:9">
+      <c r="E13" t="s">
+        <v>104</v>
+      </c>
       <c r="I13" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:9">
+      <c r="E14" t="s">
+        <v>105</v>
+      </c>
       <c r="I14" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -847,7 +884,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="G14" sqref="G14:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1155,31 +1192,49 @@
       </c>
     </row>
     <row r="14" spans="1:12">
+      <c r="G14" t="s">
+        <v>97</v>
+      </c>
       <c r="L14" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:12">
+      <c r="G15" t="s">
+        <v>98</v>
+      </c>
       <c r="L15" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:12">
+      <c r="G16" t="s">
+        <v>99</v>
+      </c>
       <c r="L16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="12:12">
+    <row r="17" spans="7:12">
+      <c r="G17" t="s">
+        <v>100</v>
+      </c>
       <c r="L17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="12:12">
+    <row r="18" spans="7:12">
+      <c r="G18" t="s">
+        <v>101</v>
+      </c>
       <c r="L18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="12:12">
+    <row r="19" spans="7:12">
+      <c r="G19" t="s">
+        <v>102</v>
+      </c>
       <c r="L19" t="s">
         <v>75</v>
       </c>
@@ -1917,7 +1972,7 @@
   <sheetPr codeName="Лист5"/>
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="V4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>

</xml_diff>